<commit_message>
Dossier : relecture en cours
</commit_message>
<xml_diff>
--- a/dossiers/Données finales/Answer - Longueur auteurs.xlsx
+++ b/dossiers/Données finales/Answer - Longueur auteurs.xlsx
@@ -1,28 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\dossiers\Données finales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23F7F1F-D02C-4EF6-AEBF-FB375B3997DB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76668DA4-F4D5-4D52-A7AD-905CA9E96331}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NB_AUTHORS NB LENGTHS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -2379,7 +2372,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4241,8 +4234,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4568,8 +4561,8 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S68" sqref="S68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4599,7 +4592,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6">
-        <f>D2/C2</f>
+        <f t="shared" ref="B2:B47" si="0">D2/C2</f>
         <v>15.704183704504748</v>
       </c>
       <c r="C2" s="5">
@@ -4609,7 +4602,7 @@
         <v>929405</v>
       </c>
       <c r="E2" s="8">
-        <f>C2/85531</f>
+        <f t="shared" ref="E2:E47" si="1">C2/85531</f>
         <v>0.69193625702961503</v>
       </c>
     </row>
@@ -4618,7 +4611,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6">
-        <f>D3/C3</f>
+        <f t="shared" si="0"/>
         <v>14.530702118820107</v>
       </c>
       <c r="C3" s="5">
@@ -4628,7 +4621,7 @@
         <v>174877</v>
       </c>
       <c r="E3" s="8">
-        <f>C3/85531</f>
+        <f t="shared" si="1"/>
         <v>0.14070921654137097</v>
       </c>
     </row>
@@ -4637,7 +4630,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6">
-        <f>D4/C4</f>
+        <f t="shared" si="0"/>
         <v>15.133333333333333</v>
       </c>
       <c r="C4" s="5">
@@ -4647,7 +4640,7 @@
         <v>91027</v>
       </c>
       <c r="E4" s="8">
-        <f>C4/85531</f>
+        <f t="shared" si="1"/>
         <v>7.0325379102313776E-2</v>
       </c>
     </row>
@@ -4656,7 +4649,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6">
-        <f>D5/C5</f>
+        <f t="shared" si="0"/>
         <v>15.61570996978852</v>
       </c>
       <c r="C5" s="5">
@@ -4666,7 +4659,7 @@
         <v>51688</v>
       </c>
       <c r="E5" s="8">
-        <f>C5/85531</f>
+        <f t="shared" si="1"/>
         <v>3.869941892413277E-2</v>
       </c>
     </row>
@@ -4675,7 +4668,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6">
-        <f>D6/C6</f>
+        <f t="shared" si="0"/>
         <v>16.078186968838526</v>
       </c>
       <c r="C6" s="5">
@@ -4685,7 +4678,7 @@
         <v>28378</v>
       </c>
       <c r="E6" s="8">
-        <f>C6/85531</f>
+        <f t="shared" si="1"/>
         <v>2.0635792870421252E-2</v>
       </c>
     </row>
@@ -4694,7 +4687,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="6">
-        <f>D7/C7</f>
+        <f t="shared" si="0"/>
         <v>16.376525821596243</v>
       </c>
       <c r="C7" s="5">
@@ -4704,7 +4697,7 @@
         <v>17441</v>
       </c>
       <c r="E7" s="8">
-        <f>C7/85531</f>
+        <f t="shared" si="1"/>
         <v>1.2451625726344834E-2</v>
       </c>
     </row>
@@ -4713,7 +4706,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="6">
-        <f>D8/C8</f>
+        <f t="shared" si="0"/>
         <v>17.211901306240929</v>
       </c>
       <c r="C8" s="5">
@@ -4723,7 +4716,7 @@
         <v>11859</v>
       </c>
       <c r="E8" s="8">
-        <f>C8/85531</f>
+        <f t="shared" si="1"/>
         <v>8.0555588032409295E-3</v>
       </c>
     </row>
@@ -4732,7 +4725,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="6">
-        <f>D9/C9</f>
+        <f t="shared" si="0"/>
         <v>17.281927710843373</v>
       </c>
       <c r="C9" s="5">
@@ -4742,7 +4735,7 @@
         <v>7172</v>
       </c>
       <c r="E9" s="7">
-        <f>C9/85531</f>
+        <f t="shared" si="1"/>
         <v>4.8520419497024474E-3</v>
       </c>
     </row>
@@ -4751,7 +4744,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <f>D10/C10</f>
+        <f t="shared" si="0"/>
         <v>17.887218045112782</v>
       </c>
       <c r="C10">
@@ -4761,7 +4754,7 @@
         <v>4758</v>
       </c>
       <c r="E10" s="4">
-        <f>C10/85531</f>
+        <f t="shared" si="1"/>
         <v>3.1099835147490383E-3</v>
       </c>
     </row>
@@ -4770,7 +4763,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <f>D11/C11</f>
+        <f t="shared" si="0"/>
         <v>17.251256281407034</v>
       </c>
       <c r="C11">
@@ -4780,7 +4773,7 @@
         <v>3433</v>
       </c>
       <c r="E11" s="4">
-        <f>C11/85531</f>
+        <f t="shared" si="1"/>
         <v>2.3266418023874386E-3</v>
       </c>
     </row>
@@ -4789,7 +4782,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <f>D12/C12</f>
+        <f t="shared" si="0"/>
         <v>16.125</v>
       </c>
       <c r="C12">
@@ -4799,7 +4792,7 @@
         <v>2064</v>
       </c>
       <c r="E12" s="4">
-        <f>C12/85531</f>
+        <f t="shared" si="1"/>
         <v>1.4965334206311163E-3</v>
       </c>
     </row>
@@ -4808,7 +4801,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <f>D13/C13</f>
+        <f t="shared" si="0"/>
         <v>15.695238095238095</v>
       </c>
       <c r="C13">
@@ -4818,7 +4811,7 @@
         <v>1648</v>
       </c>
       <c r="E13" s="4">
-        <f>C13/85531</f>
+        <f t="shared" si="1"/>
         <v>1.2276250716114624E-3</v>
       </c>
     </row>
@@ -4827,7 +4820,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <f>D14/C14</f>
+        <f t="shared" si="0"/>
         <v>16.863636363636363</v>
       </c>
       <c r="C14">
@@ -4837,7 +4830,7 @@
         <v>1113</v>
       </c>
       <c r="E14" s="4">
-        <f>C14/85531</f>
+        <f t="shared" si="1"/>
         <v>7.7165004501291931E-4</v>
       </c>
     </row>
@@ -4846,7 +4839,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <f>D15/C15</f>
+        <f t="shared" si="0"/>
         <v>16.068965517241381</v>
       </c>
       <c r="C15">
@@ -4856,7 +4849,7 @@
         <v>932</v>
       </c>
       <c r="E15" s="4">
-        <f>C15/85531</f>
+        <f t="shared" si="1"/>
         <v>6.7811670622347454E-4</v>
       </c>
     </row>
@@ -4865,7 +4858,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <f>D16/C16</f>
+        <f t="shared" si="0"/>
         <v>16.511627906976745</v>
       </c>
       <c r="C16">
@@ -4875,7 +4868,7 @@
         <v>710</v>
       </c>
       <c r="E16" s="4">
-        <f>C16/85531</f>
+        <f t="shared" si="1"/>
         <v>5.0274169599326564E-4</v>
       </c>
     </row>
@@ -4884,7 +4877,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <f>D17/C17</f>
+        <f t="shared" si="0"/>
         <v>18.233333333333334</v>
       </c>
       <c r="C17">
@@ -4894,7 +4887,7 @@
         <v>547</v>
       </c>
       <c r="E17" s="4">
-        <f>C17/85531</f>
+        <f t="shared" si="1"/>
         <v>3.5075002046041785E-4</v>
       </c>
     </row>
@@ -4903,7 +4896,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <f>D18/C18</f>
+        <f t="shared" si="0"/>
         <v>15.625</v>
       </c>
       <c r="C18">
@@ -4913,7 +4906,7 @@
         <v>500</v>
       </c>
       <c r="E18" s="4">
-        <f>C18/85531</f>
+        <f t="shared" si="1"/>
         <v>3.7413335515777907E-4</v>
       </c>
     </row>
@@ -4922,7 +4915,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <f>D19/C19</f>
+        <f t="shared" si="0"/>
         <v>14.9375</v>
       </c>
       <c r="C19">
@@ -4932,7 +4925,7 @@
         <v>239</v>
       </c>
       <c r="E19" s="4">
-        <f>C19/85531</f>
+        <f t="shared" si="1"/>
         <v>1.8706667757888954E-4</v>
       </c>
     </row>
@@ -4941,7 +4934,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <f>D20/C20</f>
+        <f t="shared" si="0"/>
         <v>16.666666666666668</v>
       </c>
       <c r="C20">
@@ -4951,7 +4944,7 @@
         <v>250</v>
       </c>
       <c r="E20" s="4">
-        <f>C20/85531</f>
+        <f t="shared" si="1"/>
         <v>1.7537501023020893E-4</v>
       </c>
     </row>
@@ -4960,7 +4953,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <f>D21/C21</f>
+        <f t="shared" si="0"/>
         <v>20.888888888888889</v>
       </c>
       <c r="C21">
@@ -4970,7 +4963,7 @@
         <v>376</v>
       </c>
       <c r="E21" s="4">
-        <f>C21/85531</f>
+        <f t="shared" si="1"/>
         <v>2.1045001227625073E-4</v>
       </c>
     </row>
@@ -4979,7 +4972,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <f>D22/C22</f>
+        <f t="shared" si="0"/>
         <v>13.166666666666666</v>
       </c>
       <c r="C22">
@@ -4989,7 +4982,7 @@
         <v>158</v>
       </c>
       <c r="E22" s="4">
-        <f>C22/85531</f>
+        <f t="shared" si="1"/>
         <v>1.4030000818416715E-4</v>
       </c>
     </row>
@@ -4998,7 +4991,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <f>D23/C23</f>
+        <f t="shared" si="0"/>
         <v>19.875</v>
       </c>
       <c r="C23">
@@ -5008,7 +5001,7 @@
         <v>159</v>
       </c>
       <c r="E23" s="4">
-        <f>C23/85531</f>
+        <f t="shared" si="1"/>
         <v>9.3533338789444768E-5</v>
       </c>
     </row>
@@ -5017,7 +5010,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <f>D24/C24</f>
+        <f t="shared" si="0"/>
         <v>15.888888888888889</v>
       </c>
       <c r="C24">
@@ -5027,7 +5020,7 @@
         <v>143</v>
       </c>
       <c r="E24" s="4">
-        <f>C24/85531</f>
+        <f t="shared" si="1"/>
         <v>1.0522500613812536E-4</v>
       </c>
     </row>
@@ -5036,7 +5029,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <f>D25/C25</f>
+        <f t="shared" si="0"/>
         <v>19.2</v>
       </c>
       <c r="C25">
@@ -5046,7 +5039,7 @@
         <v>96</v>
       </c>
       <c r="E25" s="4">
-        <f>C25/85531</f>
+        <f t="shared" si="1"/>
         <v>5.845833674340298E-5</v>
       </c>
     </row>
@@ -5055,7 +5048,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <f>D26/C26</f>
+        <f t="shared" si="0"/>
         <v>17.714285714285715</v>
       </c>
       <c r="C26">
@@ -5065,7 +5058,7 @@
         <v>124</v>
       </c>
       <c r="E26" s="4">
-        <f>C26/85531</f>
+        <f t="shared" si="1"/>
         <v>8.1841671440764172E-5</v>
       </c>
     </row>
@@ -5074,7 +5067,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <f>D27/C27</f>
+        <f t="shared" si="0"/>
         <v>18.333333333333332</v>
       </c>
       <c r="C27">
@@ -5084,7 +5077,7 @@
         <v>110</v>
       </c>
       <c r="E27" s="4">
-        <f>C27/85531</f>
+        <f t="shared" si="1"/>
         <v>7.0150004092083576E-5</v>
       </c>
     </row>
@@ -5093,7 +5086,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <f>D28/C28</f>
+        <f t="shared" si="0"/>
         <v>16.2</v>
       </c>
       <c r="C28">
@@ -5103,7 +5096,7 @@
         <v>81</v>
       </c>
       <c r="E28" s="4">
-        <f>C28/85531</f>
+        <f t="shared" si="1"/>
         <v>5.845833674340298E-5</v>
       </c>
       <c r="H28" s="3">
@@ -5118,7 +5111,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <f>D29/C29</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C29">
@@ -5128,7 +5121,7 @@
         <v>40</v>
       </c>
       <c r="E29" s="4">
-        <f>C29/85531</f>
+        <f t="shared" si="1"/>
         <v>2.3383334697361192E-5</v>
       </c>
       <c r="H29" s="3">
@@ -5143,7 +5136,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <f>D30/C30</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C30">
@@ -5153,7 +5146,7 @@
         <v>51</v>
       </c>
       <c r="E30" s="4">
-        <f>C30/85531</f>
+        <f t="shared" si="1"/>
         <v>3.5075002046041788E-5</v>
       </c>
       <c r="H30" s="3">
@@ -5168,7 +5161,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <f>D31/C31</f>
+        <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
       <c r="C31">
@@ -5178,7 +5171,7 @@
         <v>45</v>
       </c>
       <c r="E31" s="4">
-        <f>C31/85531</f>
+        <f t="shared" si="1"/>
         <v>2.3383334697361192E-5</v>
       </c>
     </row>
@@ -5187,7 +5180,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <f>D32/C32</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C32">
@@ -5197,7 +5190,7 @@
         <v>18</v>
       </c>
       <c r="E32" s="4">
-        <f>C32/85531</f>
+        <f t="shared" si="1"/>
         <v>2.3383334697361192E-5</v>
       </c>
     </row>
@@ -5206,7 +5199,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <f>D33/C33</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C33">
@@ -5216,7 +5209,7 @@
         <v>18</v>
       </c>
       <c r="E33" s="4">
-        <f>C33/85531</f>
+        <f t="shared" si="1"/>
         <v>1.1691667348680596E-5</v>
       </c>
     </row>
@@ -5225,7 +5218,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <f>D34/C34</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C34">
@@ -5235,7 +5228,7 @@
         <v>5</v>
       </c>
       <c r="E34" s="4">
-        <f>C34/85531</f>
+        <f t="shared" si="1"/>
         <v>1.1691667348680596E-5</v>
       </c>
     </row>
@@ -5244,7 +5237,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <f>D35/C35</f>
+        <f t="shared" si="0"/>
         <v>16.5</v>
       </c>
       <c r="C35">
@@ -5254,7 +5247,7 @@
         <v>33</v>
       </c>
       <c r="E35" s="4">
-        <f>C35/85531</f>
+        <f t="shared" si="1"/>
         <v>2.3383334697361192E-5</v>
       </c>
     </row>
@@ -5263,7 +5256,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <f>D36/C36</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C36">
@@ -5273,7 +5266,7 @@
         <v>19</v>
       </c>
       <c r="E36" s="4">
-        <f>C36/85531</f>
+        <f t="shared" si="1"/>
         <v>1.1691667348680596E-5</v>
       </c>
     </row>
@@ -5282,7 +5275,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <f>D37/C37</f>
+        <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
       <c r="C37">
@@ -5292,7 +5285,7 @@
         <v>27</v>
       </c>
       <c r="E37" s="4">
-        <f>C37/85531</f>
+        <f t="shared" si="1"/>
         <v>2.3383334697361192E-5</v>
       </c>
     </row>
@@ -5301,7 +5294,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="1">
-        <f>D38/C38</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C38">
@@ -5311,7 +5304,7 @@
         <v>20</v>
       </c>
       <c r="E38" s="4">
-        <f>C38/85531</f>
+        <f t="shared" si="1"/>
         <v>1.1691667348680596E-5</v>
       </c>
     </row>
@@ -5320,7 +5313,7 @@
         <v>40</v>
       </c>
       <c r="B39" s="1">
-        <f>D39/C39</f>
+        <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="C39">
@@ -5330,7 +5323,7 @@
         <v>19</v>
       </c>
       <c r="E39" s="4">
-        <f>C39/85531</f>
+        <f t="shared" si="1"/>
         <v>2.3383334697361192E-5</v>
       </c>
     </row>
@@ -5339,7 +5332,7 @@
         <v>44</v>
       </c>
       <c r="B40" s="1">
-        <f>D40/C40</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C40">
@@ -5349,7 +5342,7 @@
         <v>15</v>
       </c>
       <c r="E40" s="4">
-        <f>C40/85531</f>
+        <f t="shared" si="1"/>
         <v>1.1691667348680596E-5</v>
       </c>
     </row>
@@ -5358,7 +5351,7 @@
         <v>45</v>
       </c>
       <c r="B41" s="1">
-        <f>D41/C41</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C41">
@@ -5368,7 +5361,7 @@
         <v>12</v>
       </c>
       <c r="E41" s="4">
-        <f>C41/85531</f>
+        <f t="shared" si="1"/>
         <v>1.1691667348680596E-5</v>
       </c>
     </row>
@@ -5377,7 +5370,7 @@
         <v>47</v>
       </c>
       <c r="B42" s="1">
-        <f>D42/C42</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C42">
@@ -5387,7 +5380,7 @@
         <v>23</v>
       </c>
       <c r="E42" s="4">
-        <f>C42/85531</f>
+        <f t="shared" si="1"/>
         <v>1.1691667348680596E-5</v>
       </c>
     </row>
@@ -5396,7 +5389,7 @@
         <v>55</v>
       </c>
       <c r="B43" s="1">
-        <f>D43/C43</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C43">
@@ -5406,7 +5399,7 @@
         <v>19</v>
       </c>
       <c r="E43" s="4">
-        <f>C43/85531</f>
+        <f t="shared" si="1"/>
         <v>1.1691667348680596E-5</v>
       </c>
     </row>
@@ -5415,7 +5408,7 @@
         <v>58</v>
       </c>
       <c r="B44" s="1">
-        <f>D44/C44</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C44">
@@ -5425,7 +5418,7 @@
         <v>10</v>
       </c>
       <c r="E44" s="4">
-        <f>C44/85531</f>
+        <f t="shared" si="1"/>
         <v>1.1691667348680596E-5</v>
       </c>
     </row>
@@ -5434,7 +5427,7 @@
         <v>61</v>
       </c>
       <c r="B45" s="1">
-        <f>D45/C45</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C45">
@@ -5444,7 +5437,7 @@
         <v>14</v>
       </c>
       <c r="E45" s="4">
-        <f>C45/85531</f>
+        <f t="shared" si="1"/>
         <v>1.1691667348680596E-5</v>
       </c>
     </row>
@@ -5453,7 +5446,7 @@
         <v>62</v>
       </c>
       <c r="B46" s="1">
-        <f>D46/C46</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C46">
@@ -5463,7 +5456,7 @@
         <v>14</v>
       </c>
       <c r="E46" s="4">
-        <f>C46/85531</f>
+        <f t="shared" si="1"/>
         <v>1.1691667348680596E-5</v>
       </c>
     </row>
@@ -5472,7 +5465,7 @@
         <v>147</v>
       </c>
       <c r="B47" s="1">
-        <f>D47/C47</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C47">
@@ -5482,7 +5475,7 @@
         <v>6</v>
       </c>
       <c r="E47" s="4">
-        <f>C47/85531</f>
+        <f t="shared" si="1"/>
         <v>1.1691667348680596E-5</v>
       </c>
     </row>

</xml_diff>